<commit_message>
metric 5 6 graph updated
</commit_message>
<xml_diff>
--- a/correlation/correlation 5 and 6/correlation 5 and 6 - commons-lang.xlsx
+++ b/correlation/correlation 5 and 6/correlation 5 and 6 - commons-lang.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shalin_patel/Downloads/soen6611-measurement-metrics/correlation/correlation 5 and 6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A96D351-7160-5048-B27D-2A003489DF52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1E12CB-AF5D-EC4B-B60A-2A5780CFDDA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2465,7 +2465,7 @@
   <dimension ref="A3:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2655,6 +2655,10 @@
       </c>
       <c r="C16" s="7">
         <v>4.7826294896934338E-2</v>
+      </c>
+      <c r="D16">
+        <f>CORREL(B16:B21,C16:C21)</f>
+        <v>-7.3353082841378703E-2</v>
       </c>
       <c r="F16"/>
     </row>

</xml_diff>